<commit_message>
Changed sum of IC-capacity to maximum IC-capacity per month
</commit_message>
<xml_diff>
--- a/Arima_results.xlsx
+++ b/Arima_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8792.83914958519</v>
+        <v>340.6502365674644</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9327.606891159847</v>
+        <v>380.1709986241312</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7229.133841866047</v>
+        <v>466.4927275488926</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10082.08518654623</v>
+        <v>442.3999701996131</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7308.948948967987</v>
+        <v>282.3504441540706</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7575.046749351333</v>
+        <v>495.8227692109853</v>
       </c>
     </row>
     <row r="8">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6913.448632829081</v>
+        <v>503.5020521473747</v>
       </c>
     </row>
     <row r="9">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>11396.07798331627</v>
+        <v>534.2329043762988</v>
       </c>
     </row>
     <row r="10">
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10547.68173539755</v>
+        <v>508.2810796541641</v>
       </c>
     </row>
     <row r="11">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10544.02610653918</v>
+        <v>437.3966666263567</v>
       </c>
     </row>
     <row r="12">
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9760.252951835922</v>
+        <v>337.4029434358142</v>
       </c>
     </row>
     <row r="13">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7588.781365892567</v>
+        <v>305.4142891313475</v>
       </c>
     </row>
     <row r="14">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7840.046985186198</v>
+        <v>284.42040542354</v>
       </c>
     </row>
     <row r="15">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>7068.647976460167</v>
+        <v>502.5108446169883</v>
       </c>
     </row>
     <row r="16">
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6823.346520852231</v>
+        <v>349.3221794436784</v>
       </c>
     </row>
     <row r="17">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5118.65466338364</v>
+        <v>216.557585124399</v>
       </c>
     </row>
     <row r="18">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4285.147798826442</v>
+        <v>225.4852715383226</v>
       </c>
     </row>
     <row r="19">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>33736.09963386013</v>
+        <v>368.253494630708</v>
       </c>
     </row>
     <row r="20">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5587.465005039627</v>
+        <v>224.6647038751593</v>
       </c>
     </row>
     <row r="21">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7861.296462112718</v>
+        <v>309.9864289648673</v>
       </c>
     </row>
     <row r="22">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5620.559224469658</v>
+        <v>307.4330988189717</v>
       </c>
     </row>
     <row r="23">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6731.958831830265</v>
+        <v>352.8185281751925</v>
       </c>
     </row>
     <row r="24">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>7208.131170978689</v>
+        <v>304.0039148229766</v>
       </c>
     </row>
     <row r="25">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5015.607150299804</v>
+        <v>201.0344671326881</v>
       </c>
     </row>
     <row r="26">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>10507.44675992797</v>
+        <v>361.3978834513393</v>
       </c>
     </row>
     <row r="27">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4671.21731333604</v>
+        <v>265.2880644961264</v>
       </c>
     </row>
     <row r="28">
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>6322.464981094636</v>
+        <v>282.6231269891917</v>
       </c>
     </row>
     <row r="29">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5377.849629217556</v>
+        <v>252.5436773803101</v>
       </c>
     </row>
     <row r="30">
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>6807.884296556252</v>
+        <v>334.024038593734</v>
       </c>
     </row>
     <row r="31">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>7840.407323988021</v>
+        <v>349.837404554086</v>
       </c>
     </row>
     <row r="32">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5019.401340070582</v>
+        <v>307.9019510352074</v>
       </c>
     </row>
     <row r="33">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>29920.93986360385</v>
+        <v>189.6693852564502</v>
       </c>
     </row>
     <row r="34">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4912.352057218353</v>
+        <v>365.4000240489517</v>
       </c>
     </row>
     <row r="35">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4633.951771647609</v>
+        <v>287.6846542207747</v>
       </c>
     </row>
     <row r="36">
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5124.835797236787</v>
+        <v>201.3461906860068</v>
       </c>
     </row>
     <row r="37">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>6380.18186799861</v>
+        <v>438.1491704926532</v>
       </c>
     </row>
     <row r="38">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>7412.798244442595</v>
+        <v>439.0007528979557</v>
       </c>
     </row>
     <row r="39">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>4829.070842072184</v>
+        <v>393.599403680087</v>
       </c>
     </row>
     <row r="40">
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>53252.62997232969</v>
+        <v>311.2395037424493</v>
       </c>
     </row>
     <row r="41">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>5441.837043396114</v>
+        <v>222.0121201869233</v>
       </c>
     </row>
     <row r="42">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4776.44202147303</v>
+        <v>380.9072746760096</v>
       </c>
     </row>
     <row r="43">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4977.301157020532</v>
+        <v>290.6370800647912</v>
       </c>
     </row>
     <row r="44">
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>5661.154591094613</v>
+        <v>365.991398300569</v>
       </c>
     </row>
     <row r="45">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>6060.418825030786</v>
+        <v>399.9812871821335</v>
       </c>
     </row>
     <row r="46">
@@ -887,117 +887,107 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>6006.596328862436</v>
+        <v>566.9913101431812</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>(6, 0, 3)</t>
+          <t>(6, 0, 5)</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>451323.822197461</v>
+        <v>364.2436063050155</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>(6, 0, 5)</t>
+          <t>(6, 0, 6)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>5211.027258155763</v>
+        <v>229.4288501838379</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>(6, 0, 6)</t>
+          <t>(6, 0, 7)</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>5748.566331706749</v>
+        <v>248.4104850046107</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>(6, 0, 7)</t>
+          <t>(7, 0, 0)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4846.019109593516</v>
+        <v>371.2264591495643</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>(7, 0, 0)</t>
+          <t>(7, 0, 1)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>9058.764212959728</v>
+        <v>348.7460421366534</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>(7, 0, 1)</t>
+          <t>(7, 0, 2)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>7080.984045778459</v>
+        <v>344.818675737992</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>(7, 0, 2)</t>
+          <t>(7, 0, 3)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>8494.968807506308</v>
+        <v>385.7467845371036</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>(7, 0, 3)</t>
+          <t>(7, 0, 5)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>8792.901205168233</v>
+        <v>222.9846743578483</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>(7, 0, 5)</t>
+          <t>(7, 0, 6)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>5263.159801763112</v>
+        <v>281.0098902576678</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>(7, 0, 6)</t>
+          <t>(7, 0, 7)</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>5161.073441286589</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>(7, 0, 7)</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>5082.503658351181</v>
+        <v>242.0748495274166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>